<commit_message>
Código pruebas expansor GPIO (no funciona de momento)
</commit_message>
<xml_diff>
--- a/SW/docs/pin_map.xlsx
+++ b/SW/docs/pin_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabian\Desktop\workspace\UPM\Laboratorio\ISE\Bloque_II\ise_grupo_l7\SW\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36F2A9CC-F888-4BD8-8647-B728989D1D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD12E6C-D8C2-47BA-B310-B523E84B0EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F4287D60-1757-4D2A-9393-44E16816D05C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>Pin NUCLEO</t>
   </si>
@@ -181,8 +181,24 @@
     <t>PB9</t>
   </si>
   <si>
+    <t>PRINTF</t>
+  </si>
+  <si>
+    <t>PB3</t>
+  </si>
+  <si>
+    <t>PC8</t>
+  </si>
+  <si>
     <t>POSICION
-I2C1</t>
+I2C1
+(Test)</t>
+  </si>
+  <si>
+    <t>Prueba I2C</t>
+  </si>
+  <si>
+    <t>P00</t>
   </si>
 </sst>
 </file>
@@ -220,7 +236,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -244,28 +260,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thick">
@@ -449,95 +443,105 @@
       <bottom style="thick">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -888,13 +892,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B9EBC1D-47E5-4E1D-B745-0D88080E3EAC}">
-  <dimension ref="B1:G21"/>
+  <dimension ref="B1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -906,7 +916,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="18" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -920,7 +930,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="9"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
@@ -932,7 +942,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="9"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
@@ -944,7 +954,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="9"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
@@ -956,7 +966,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="10"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="6" t="s">
         <v>6</v>
       </c>
@@ -968,177 +978,202 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="13"/>
-      <c r="C9" s="16" t="s">
+      <c r="B9" s="28"/>
+      <c r="C9" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="26"/>
+      <c r="G10" s="17"/>
     </row>
     <row r="11" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="9"/>
-      <c r="C11" s="18" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="9"/>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="19"/>
+      <c r="C12" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="9"/>
-      <c r="C13" s="18" t="s">
+      <c r="B13" s="19"/>
+      <c r="C13" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="9"/>
-      <c r="C14" s="18" t="s">
+      <c r="B14" s="19"/>
+      <c r="C14" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="9"/>
-      <c r="C15" s="18" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="9"/>
-      <c r="C16" s="18" t="s">
+      <c r="B16" s="19"/>
+      <c r="C16" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="9"/>
-      <c r="C17" s="18" t="s">
+    <row r="17" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="19"/>
+      <c r="C17" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="13" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="10"/>
-      <c r="C18" s="16" t="s">
+      <c r="F17" s="17"/>
+    </row>
+    <row r="18" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="20"/>
+      <c r="C18" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="11" t="s">
+    <row r="19" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="23"/>
+      <c r="D19" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="25"/>
+    </row>
+    <row r="20" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="24"/>
-    </row>
-    <row r="20" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="23"/>
-      <c r="C20" s="16" t="s">
+      <c r="E20" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="22"/>
+      <c r="C21" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D21" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="25"/>
-    </row>
-    <row r="21" spans="2:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="E21" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B18"/>
-    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B20:B21"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E9 E19:E1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  <conditionalFormatting sqref="E20:E1048576 E1:E9">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>